<commit_message>
close to final on bar charts
</commit_message>
<xml_diff>
--- a/data/jho_correlation_data.xlsx
+++ b/data/jho_correlation_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="8532" windowWidth="23040" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" windowHeight="8532" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Burrows MP" sheetId="1" r:id="rId1"/>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>PAS</t>
+  </si>
+  <si>
+    <t>average(</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="topLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -1378,6 +1381,12 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="1">
+        <f>AVERAGE(B2:B21)</f>
+        <v>3.666665</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:N21">
@@ -5461,7 +5470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="topLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
starting to figure out anova's  some data issues still
</commit_message>
<xml_diff>
--- a/data/jho_correlation_data.xlsx
+++ b/data/jho_correlation_data.xlsx
@@ -529,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="topLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
@@ -1383,10 +1383,7 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23">
-      <c r="B23" s="1">
-        <f>AVERAGE(B2:B21)</f>
-        <v>3.666665</v>
-      </c>
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:N21">

</xml_diff>